<commit_message>
data processing and plotting work done
</commit_message>
<xml_diff>
--- a/Preliminary tests (semi-valid)/compression_resistance_#12_test.xlsx
+++ b/Preliminary tests (semi-valid)/compression_resistance_#12_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Postgrad\6. Projects\electro-mech-stretcher\code\electromech-stretcher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Postgrad\6. Projects\electro-mech-stretcher\code\electromech-stretcher\Preliminary tests (semi-valid)\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="compression_resistance_#12_test" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -600,38 +600,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -662,20 +631,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'compression_resistance_#12_test'!$E$2:$E$41</c:f>
@@ -944,30 +899,72 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-73875520"/>
-        <c:axId val="-73869536"/>
+        <c:axId val="1848179312"/>
+        <c:axId val="1848181488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-73875520"/>
+        <c:axId val="1848179312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Compressive Strain</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1005,12 +1002,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-73869536"/>
+        <c:crossAx val="1848181488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-73869536"/>
+        <c:axId val="1848181488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1030,6 +1027,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Resistance [Ohm]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1067,7 +1120,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-73875520"/>
+        <c:crossAx val="1848179312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1682,8 +1735,8 @@
       <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>194310</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1234440</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
@@ -1972,8 +2025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1982,9 +2035,10 @@
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.44140625" customWidth="1"/>
-    <col min="5" max="5" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="37.5546875" customWidth="1"/>
+    <col min="7" max="7" width="39" customWidth="1"/>
+    <col min="8" max="8" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>